<commit_message>
working all groups organised but last one
</commit_message>
<xml_diff>
--- a/output_combinations_optimized.xlsx
+++ b/output_combinations_optimized.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,34 +499,28 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>bags</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>240000</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Group 2</t>
+      <c r="A4" s="2" t="inlineStr"/>
+      <c r="B4" s="2" t="inlineStr"/>
+      <c r="C4" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>23542</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>wings</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>80000</v>
+        <v>240000</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -529,105 +530,93 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4567</v>
+        <v>23542</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>suspension</t>
+          <t>wings</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>200000</v>
+        <v>80000</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Group 3</t>
+          <t>Group 2</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>45</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>rice bags</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>120000</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Group 3</t>
+      <c r="A7" s="2" t="inlineStr"/>
+      <c r="B7" s="2" t="inlineStr"/>
+      <c r="C7" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>123123</v>
+        <v>4567</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>suspension</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>120000</v>
+        <v>200000</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Group 4</t>
+          <t>Group 3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3457</v>
+        <v>45</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>snake</t>
+          <t>rice bags</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>90000</v>
+        <v>120000</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Group 4</t>
+          <t>Group 3</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>23452</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Screens</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>80000</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Group 4</t>
+      <c r="A10" s="2" t="inlineStr"/>
+      <c r="B10" s="2" t="inlineStr"/>
+      <c r="C10" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>123123</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>bottle</t>
+          <t>Dog</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>30000</v>
+        <v>120000</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -637,87 +626,81 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>567</v>
+        <v>3457</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>boots</t>
+          <t>snake</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>80000</v>
+        <v>90000</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Group 5</t>
+          <t>Group 4</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>345</v>
+        <v>23452</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Weights</t>
+          <t>Screens</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>65000</v>
+        <v>80000</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Group 5</t>
+          <t>Group 4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>watches</t>
+          <t>bottle</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Group 5</t>
+          <t>Group 4</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>234</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>mouse</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>60000</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Group 5</t>
+      <c r="A15" s="2" t="inlineStr"/>
+      <c r="B15" s="2" t="inlineStr"/>
+      <c r="C15" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>24</v>
+        <v>567</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Grape</t>
+          <t>boots</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>40000</v>
+        <v>80000</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -727,29 +710,29 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2131</v>
+        <v>345</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Weights</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>60000</v>
+        <v>65000</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Group 6</t>
+          <t>Group 5</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>576</v>
+        <v>74</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>hippo</t>
+          <t>watches</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -757,17 +740,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Group 6</t>
+          <t>Group 5</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>tea bags</t>
+          <t>mouse</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -775,17 +758,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Group 6</t>
+          <t>Group 5</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2435345</v>
+        <v>24</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>spoons</t>
+          <t>Grape</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -793,7 +776,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Group 6</t>
+          <t>Group 5</t>
         </is>
       </c>
     </row>
@@ -807,93 +790,87 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>320000</v>
+        <v>15000</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Group 7</t>
+          <t>Group 5</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>456</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>yoyo</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>320000</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Group 8</t>
+      <c r="A22" s="2" t="inlineStr"/>
+      <c r="B22" s="2" t="inlineStr"/>
+      <c r="C22" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 5</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>4363</v>
+        <v>2131</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>rags</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>320000</v>
+        <v>60000</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Group 9</t>
+          <t>Group 6</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>4363</v>
+        <v>576</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>rags</t>
+          <t>hippo</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>210000</v>
+        <v>60000</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Group 10</t>
+          <t>Group 6</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>56</v>
+        <v>245</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>hats</t>
+          <t>tea bags</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>320000</v>
+        <v>60000</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Group 11</t>
+          <t>Group 6</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>56</v>
+        <v>2435345</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>hats</t>
+          <t>spoons</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -901,43 +878,253 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Group 12</t>
+          <t>Group 6</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
+        <v>4363</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>rags</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Group 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr"/>
+      <c r="B28" s="2" t="inlineStr"/>
+      <c r="C28" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>4363</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>rags</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Group 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr"/>
+      <c r="B30" s="2" t="inlineStr"/>
+      <c r="C30" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
         <v>456</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>yoyo</t>
         </is>
       </c>
-      <c r="C27" t="n">
-        <v>320000</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Group 13</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
+      <c r="C31" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Group 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr"/>
+      <c r="B32" s="2" t="inlineStr"/>
+      <c r="C32" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4363</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>rags</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Group 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr"/>
+      <c r="B34" s="2" t="inlineStr"/>
+      <c r="C34" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>4363</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>rags</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>95000</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Group 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>56</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>hats</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>225000</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Group 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr"/>
+      <c r="B37" s="2" t="inlineStr"/>
+      <c r="C37" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>56</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>hats</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>135000</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Group 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
         <v>456</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B39" t="inlineStr">
         <is>
           <t>yoyo</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>10000</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Group 14</t>
+      <c r="C39" t="n">
+        <v>185000</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Group 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr"/>
+      <c r="B40" s="2" t="inlineStr"/>
+      <c r="C40" s="2" t="n">
+        <v>320000</v>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>456</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>yoyo</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>145000</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Group 12</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr"/>
+      <c r="B42" s="2" t="inlineStr"/>
+      <c r="C42" s="2" t="n">
+        <v>145000</v>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>Total Group 12</t>
         </is>
       </c>
     </row>

</xml_diff>